<commit_message>
Added a new dependency to take care of the java No class found Exception
</commit_message>
<xml_diff>
--- a/com.adactin.hotelapp/target/test-classes/MasterTestData.xlsx
+++ b/com.adactin.hotelapp/target/test-classes/MasterTestData.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17127"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18528"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\efrain\Java_practice_workspace\test_automation\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\efrain\git\com.adactin.hotelapp\com.adactin.hotelapp\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16230" windowHeight="9030"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16230" windowHeight="9030" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="adactin" sheetId="1" r:id="rId1"/>
+    <sheet name="com.adactin.hotelapp" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">adactin!$A$1:$I$20</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'com.adactin.hotelapp'!$A$1:$I$20</definedName>
   </definedNames>
   <calcPr calcId="0"/>
   <extLst>
@@ -176,7 +176,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -522,7 +522,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I23"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
@@ -834,7 +834,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:I20"/>
+  <autoFilter ref="A1:I20" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>